<commit_message>
Update MADMC B19 Pregancy Outcome Estimate Tool.xlsx
</commit_message>
<xml_diff>
--- a/Phase 1/MADMC B19 Pregancy Outcome Estimate Tool.xlsx
+++ b/Phase 1/MADMC B19 Pregancy Outcome Estimate Tool.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ritesh/Desktop/parvo-b19-modeling/Phase 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531A8C0B-CB8B-1A41-81B4-D8B8AAFAEF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{234AF648-CDA1-934D-AF21-B9E79A339736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="520" windowWidth="38400" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="2" r:id="rId1"/>
@@ -19,13 +19,6 @@
     <sheet name="Data Sources" sheetId="4" r:id="rId4"/>
     <sheet name="Limitations &amp; Strengths" sheetId="5" r:id="rId5"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v2.0" hidden="1">'Base Case Estimates'!$B$47:$B$49</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">'Base Case Estimates'!$C$46</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">'Base Case Estimates'!$C$47:$C$49</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">'Base Case Estimates'!$D$46</definedName>
-    <definedName name="_xlchart.v2.4" hidden="1">'Base Case Estimates'!$D$47:$D$49</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="149">
   <si>
     <t>Number at Risk</t>
   </si>
@@ -115,9 +108,6 @@
     <t>Parameters</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.state.mn.us/data/madmc/index.html </t>
-  </si>
-  <si>
     <t>Table 1. Results for Immunity Ranges 50-100% and Infection Probabilities 0-10% (Figure 1 data)</t>
   </si>
   <si>
@@ -1236,29 +1226,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">For questions, please contact: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Margo Wheatley, PhD (jaco2580@umn.edu), or Lindsey Erickson, PhD (Lindsey.Erickson@state.mn.us)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">Last Updated: </t>
     </r>
     <r>
@@ -1515,34 +1482,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>Parvovirus B19 (B19) can lead to rare but severe outcomes among fetuses when mothers are infected in the first 20-22 weeks of pregnancy. B19 cases have recently surged in the United States (https://emergency.cdc.gov/han/2024/han00514.asp) and downstream severe fetal outcomes have been observed.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Note: This tool is under development and is </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="16"/>
-        <color rgb="FFED0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>not to be shared</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color rgb="FFED0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> outside of the Minnesota Department of Health or University of Minnesota.</t>
     </r>
   </si>
   <si>
@@ -1861,6 +1800,77 @@
       </rPr>
       <t xml:space="preserve"> This tab estimates of the number of parvovirus B19-related outcomes under a wide range of immunity and infection probability parameter values. Users can change number of expected pregnancies to obtain estimates that reflect their local population, as well as change estimates for the probability of maternal-fetal infection and the probability of severe fetal outcomes. 
 This tab uses two-way sensitivity analysis to vary two parameter values simultaneously. For a more realistic scenario, proportion of population immune varies from 25%-75% while infection probability varies from 0.5-10%. A purely hypothetical scenario evaluates all possible parameter values, ranging immunity from 0-100% and infection probability from 0-100%.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Red box</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> indicates hypothetical severe outbreak estimates of immunity and infection probability</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.sph.umn.edu/research/centers/midwest-analytics-and-disease-modeling/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">For questions, please contact: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UMN's MADMC Center at madmc@umn.edu</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Funding:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> This work was supported by cooperative agreement CDC-RFA-FT-23-0069 from the Center for Forecasting and Outbreak Analytics of the US Centers for Disease Control and Prevention. Its contents are solely the responsibility of the authors and do not necessarily represent the official views of the CDC.
+The authors have no conflicts to disclose.</t>
     </r>
   </si>
 </sst>
@@ -2065,15 +2075,6 @@
     </font>
     <font>
       <b/>
-      <u/>
-      <sz val="16"/>
-      <color rgb="FFED0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="24"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -2093,6 +2094,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="10">
@@ -2151,7 +2158,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -2344,6 +2351,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2351,7 +2438,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2561,7 +2648,7 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2573,10 +2660,10 @@
     <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2603,133 +2690,29 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2760,9 +2743,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2780,15 +2760,120 @@
     <xf numFmtId="3" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3550,13 +3635,10 @@
               <a:buFontTx/>
               <a:buNone/>
               <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr>
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -3778,7 +3860,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -5475,10 +5557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D67F48-99C5-4DBB-9139-21F0A09DC1AF}">
-  <dimension ref="B4:L44"/>
+  <dimension ref="B4:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5503,7 +5585,7 @@
     <row r="6" spans="2:12" ht="32" x14ac:dyDescent="0.2">
       <c r="B6" s="18"/>
       <c r="C6" s="79" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="90"/>
@@ -5535,9 +5617,7 @@
     </row>
     <row r="9" spans="2:12" ht="21" x14ac:dyDescent="0.2">
       <c r="B9" s="18"/>
-      <c r="C9" s="80" t="s">
-        <v>119</v>
-      </c>
+      <c r="C9" s="80"/>
       <c r="D9" s="75"/>
       <c r="E9" s="91"/>
       <c r="F9" s="91"/>
@@ -5556,7 +5636,7 @@
     <row r="11" spans="2:12" ht="66" x14ac:dyDescent="0.2">
       <c r="B11" s="18"/>
       <c r="C11" s="81" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D11" s="76"/>
       <c r="E11" s="92"/>
@@ -5584,7 +5664,7 @@
     <row r="13" spans="2:12" ht="44" x14ac:dyDescent="0.2">
       <c r="B13" s="18"/>
       <c r="C13" s="81" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D13" s="76"/>
       <c r="E13" s="92"/>
@@ -5625,7 +5705,7 @@
     <row r="16" spans="2:12" ht="21" x14ac:dyDescent="0.2">
       <c r="B16" s="18"/>
       <c r="C16" s="82" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D16" s="76"/>
       <c r="E16" s="92"/>
@@ -5640,7 +5720,7 @@
     <row r="17" spans="2:12" ht="23" x14ac:dyDescent="0.2">
       <c r="B17" s="18"/>
       <c r="C17" s="81" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D17" s="76"/>
       <c r="E17" s="92"/>
@@ -5654,7 +5734,7 @@
     <row r="18" spans="2:12" ht="23" x14ac:dyDescent="0.2">
       <c r="B18" s="18"/>
       <c r="C18" s="81" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D18" s="76"/>
       <c r="E18" s="92"/>
@@ -5668,7 +5748,7 @@
     <row r="19" spans="2:12" ht="23" x14ac:dyDescent="0.2">
       <c r="B19" s="18"/>
       <c r="C19" s="81" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D19" s="76"/>
       <c r="E19" s="92"/>
@@ -5687,7 +5767,7 @@
     <row r="21" spans="2:12" ht="110" x14ac:dyDescent="0.2">
       <c r="B21" s="18"/>
       <c r="C21" s="81" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D21" s="76"/>
       <c r="E21" s="92"/>
@@ -5771,7 +5851,7 @@
     <row r="31" spans="2:12" ht="220" x14ac:dyDescent="0.2">
       <c r="B31" s="18"/>
       <c r="C31" s="81" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D31" s="76"/>
       <c r="E31" s="92"/>
@@ -5791,7 +5871,7 @@
     <row r="33" spans="2:12" ht="154" x14ac:dyDescent="0.2">
       <c r="B33" s="18"/>
       <c r="C33" s="81" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D33" s="76"/>
       <c r="E33" s="92"/>
@@ -5819,7 +5899,7 @@
     <row r="35" spans="2:12" ht="21" x14ac:dyDescent="0.2">
       <c r="B35" s="18"/>
       <c r="C35" s="82" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D35" s="76"/>
       <c r="E35" s="92"/>
@@ -5844,7 +5924,7 @@
     <row r="38" spans="2:12" ht="44" x14ac:dyDescent="0.2">
       <c r="B38" s="11"/>
       <c r="C38" s="86" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D38" s="77"/>
       <c r="E38" s="92"/>
@@ -5861,45 +5941,59 @@
       <c r="C39" s="85"/>
       <c r="D39" s="11"/>
     </row>
-    <row r="40" spans="2:12" ht="21" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:12" ht="88" x14ac:dyDescent="0.2">
       <c r="B40" s="11"/>
-      <c r="C40" s="87" t="s">
-        <v>109</v>
+      <c r="C40" s="86" t="s">
+        <v>148</v>
       </c>
       <c r="D40" s="78"/>
     </row>
-    <row r="41" spans="2:12" ht="21" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B41" s="11"/>
-      <c r="C41" s="88" t="s">
-        <v>22</v>
-      </c>
+      <c r="C41" s="11"/>
       <c r="D41" s="11"/>
     </row>
     <row r="42" spans="2:12" ht="21" x14ac:dyDescent="0.2">
       <c r="B42" s="11"/>
-      <c r="C42" s="85"/>
+      <c r="C42" s="87" t="s">
+        <v>107</v>
+      </c>
       <c r="D42" s="11"/>
     </row>
     <row r="43" spans="2:12" ht="21" x14ac:dyDescent="0.2">
       <c r="B43" s="11"/>
-      <c r="C43" s="85" t="s">
-        <v>108</v>
+      <c r="C43" s="88" t="s">
+        <v>146</v>
       </c>
       <c r="D43" s="11"/>
     </row>
     <row r="44" spans="2:12" ht="21" x14ac:dyDescent="0.2">
       <c r="B44" s="11"/>
-      <c r="C44" s="85" t="s">
-        <v>107</v>
-      </c>
+      <c r="C44" s="85"/>
       <c r="D44" s="11"/>
     </row>
+    <row r="45" spans="2:12" ht="21" x14ac:dyDescent="0.2">
+      <c r="B45" s="11"/>
+      <c r="C45" s="85" t="s">
+        <v>106</v>
+      </c>
+      <c r="D45" s="11"/>
+    </row>
+    <row r="46" spans="2:12" ht="21" x14ac:dyDescent="0.2">
+      <c r="B46" s="11"/>
+      <c r="C46" s="85" t="s">
+        <v>147</v>
+      </c>
+      <c r="D46" s="11"/>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C41" r:id="rId1" xr:uid="{B588BF2D-A8DE-7B4A-833A-5C3F77CDF765}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5927,35 +6021,35 @@
       <c r="E1" s="27"/>
     </row>
     <row r="3" spans="2:29" ht="21" x14ac:dyDescent="0.25">
-      <c r="C3" s="136"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="136"/>
-      <c r="F3" s="136"/>
-      <c r="G3" s="136"/>
-      <c r="H3" s="136"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
       <c r="I3" s="33"/>
       <c r="J3" s="33"/>
     </row>
     <row r="4" spans="2:29" ht="21" x14ac:dyDescent="0.25">
-      <c r="B4" s="93" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="93"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="93"/>
-      <c r="H4" s="136"/>
+      <c r="B4" s="130" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="130"/>
+      <c r="D4" s="130"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="130"/>
+      <c r="G4" s="130"/>
+      <c r="H4" s="100"/>
       <c r="I4" s="33"/>
       <c r="J4" s="33"/>
     </row>
     <row r="5" spans="2:29" ht="85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="93"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
+      <c r="B5" s="130"/>
+      <c r="C5" s="130"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="130"/>
+      <c r="G5" s="130"/>
     </row>
     <row r="6" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
@@ -5979,12 +6073,12 @@
     </row>
     <row r="7" spans="2:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="137"/>
-      <c r="F7" s="137"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
       <c r="G7" s="4"/>
       <c r="H7" s="3"/>
       <c r="I7" s="4" t="s">
@@ -6001,77 +6095,77 @@
       <c r="R7" s="18"/>
     </row>
     <row r="8" spans="2:29" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="146" t="s">
+      <c r="B8" s="108" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="146" t="s">
-        <v>124</v>
-      </c>
-      <c r="D8" s="142" t="s">
+      <c r="C8" s="108" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="142" t="s">
+      <c r="E8" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="129"/>
-      <c r="G8" s="123"/>
-      <c r="H8" s="124"/>
-      <c r="I8" s="95" t="str">
+      <c r="F8" s="32"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="135" t="str">
         <f>_xlfn.CONCAT("Based on ", C9, " pregnancies in the population and historic estimates of parvovirus immunity, mother infection risk, fetal infection risk, and risk of severe fetal outcomes (Table 1), the expected number of severe fetal outcomes due to parvovirus is ",C22,". Under a best case scenario of higher immunity, lower infection rates, and lower complication rates, the number of severe fetal outcomes due to PVB19 could be as low as ", F22, ", while under a worst case scenario the number of severe fetal outcomes may be as high as ", G22, " in the population with ", C9, " pregnancies (Figure 1, Table 2).")</f>
         <v>Based on 3600000 pregnancies in the population and historic estimates of parvovirus immunity, mother infection risk, fetal infection risk, and risk of severe fetal outcomes (Table 1), the expected number of severe fetal outcomes due to parvovirus is . Under a best case scenario of higher immunity, lower infection rates, and lower complication rates, the number of severe fetal outcomes due to PVB19 could be as low as , while under a worst case scenario the number of severe fetal outcomes may be as high as  in the population with 3600000 pregnancies (Figure 1, Table 2).</v>
       </c>
-      <c r="J8" s="95"/>
-      <c r="K8" s="95"/>
-      <c r="L8" s="95"/>
-      <c r="M8" s="95"/>
-      <c r="N8" s="95"/>
-      <c r="O8" s="95"/>
-      <c r="P8" s="95"/>
+      <c r="J8" s="135"/>
+      <c r="K8" s="135"/>
+      <c r="L8" s="135"/>
+      <c r="M8" s="135"/>
+      <c r="N8" s="135"/>
+      <c r="O8" s="135"/>
+      <c r="P8" s="135"/>
       <c r="Q8" s="35"/>
       <c r="R8" s="18"/>
-      <c r="X8" s="118"/>
-      <c r="Y8" s="119"/>
-      <c r="Z8" s="119"/>
-      <c r="AA8" s="119"/>
-      <c r="AB8" s="119"/>
-      <c r="AC8" s="119"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="10"/>
+      <c r="AB8" s="10"/>
+      <c r="AC8" s="10"/>
     </row>
     <row r="9" spans="2:29" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="147" t="s">
-        <v>121</v>
-      </c>
-      <c r="C9" s="145">
+      <c r="B9" s="109" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="107">
         <v>3600000</v>
       </c>
-      <c r="D9" s="143" t="s">
+      <c r="D9" s="105" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="131"/>
-      <c r="G9" s="123"/>
-      <c r="H9" s="125"/>
-      <c r="I9" s="95"/>
-      <c r="J9" s="95"/>
-      <c r="K9" s="95"/>
-      <c r="L9" s="95"/>
-      <c r="M9" s="95"/>
-      <c r="N9" s="95"/>
-      <c r="O9" s="95"/>
-      <c r="P9" s="95"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="135"/>
+      <c r="J9" s="135"/>
+      <c r="K9" s="135"/>
+      <c r="L9" s="135"/>
+      <c r="M9" s="135"/>
+      <c r="N9" s="135"/>
+      <c r="O9" s="135"/>
+      <c r="P9" s="135"/>
       <c r="Q9" s="35"/>
       <c r="R9" s="18"/>
-      <c r="X9" s="120"/>
-      <c r="Y9" s="121"/>
-      <c r="Z9" s="121"/>
-      <c r="AA9" s="121"/>
-      <c r="AB9" s="122"/>
-      <c r="AC9" s="122"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="93"/>
+      <c r="Z9" s="93"/>
+      <c r="AA9" s="93"/>
+      <c r="AB9" s="94"/>
+      <c r="AC9" s="94"/>
     </row>
     <row r="10" spans="2:29" ht="34" x14ac:dyDescent="0.2">
       <c r="B10" s="57" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C10" s="72">
         <v>0.5</v>
@@ -6082,29 +6176,29 @@
       <c r="E10" s="73">
         <v>0.6</v>
       </c>
-      <c r="F10" s="132"/>
-      <c r="G10" s="123"/>
-      <c r="H10" s="125"/>
-      <c r="I10" s="95"/>
-      <c r="J10" s="95"/>
-      <c r="K10" s="95"/>
-      <c r="L10" s="95"/>
-      <c r="M10" s="95"/>
-      <c r="N10" s="95"/>
-      <c r="O10" s="95"/>
-      <c r="P10" s="95"/>
+      <c r="F10" s="97"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="135"/>
+      <c r="J10" s="135"/>
+      <c r="K10" s="135"/>
+      <c r="L10" s="135"/>
+      <c r="M10" s="135"/>
+      <c r="N10" s="135"/>
+      <c r="O10" s="135"/>
+      <c r="P10" s="135"/>
       <c r="Q10" s="35"/>
       <c r="R10" s="18"/>
-      <c r="X10" s="120"/>
-      <c r="Y10" s="121"/>
-      <c r="Z10" s="121"/>
-      <c r="AA10" s="121"/>
-      <c r="AB10" s="122"/>
-      <c r="AC10" s="122"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="93"/>
+      <c r="Z10" s="93"/>
+      <c r="AA10" s="93"/>
+      <c r="AB10" s="94"/>
+      <c r="AC10" s="94"/>
     </row>
     <row r="11" spans="2:29" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="57" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C11" s="72">
         <v>0.01</v>
@@ -6115,10 +6209,10 @@
       <c r="E11" s="73">
         <v>0.02</v>
       </c>
-      <c r="F11" s="132"/>
-      <c r="G11" s="126"/>
-      <c r="H11" s="124"/>
-      <c r="I11" s="124"/>
+      <c r="F11" s="97"/>
+      <c r="G11" s="95"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
@@ -6128,16 +6222,16 @@
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
       <c r="R11" s="18"/>
-      <c r="X11" s="120"/>
-      <c r="Y11" s="121"/>
-      <c r="Z11" s="121"/>
-      <c r="AA11" s="121"/>
-      <c r="AB11" s="122"/>
-      <c r="AC11" s="122"/>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="93"/>
+      <c r="Z11" s="93"/>
+      <c r="AA11" s="93"/>
+      <c r="AB11" s="94"/>
+      <c r="AC11" s="94"/>
     </row>
     <row r="12" spans="2:29" ht="50" x14ac:dyDescent="0.2">
       <c r="B12" s="57" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C12" s="72">
         <v>7.4999999999999997E-2</v>
@@ -6148,10 +6242,10 @@
       <c r="E12" s="73">
         <v>0.1</v>
       </c>
-      <c r="F12" s="132"/>
-      <c r="G12" s="126"/>
-      <c r="H12" s="124"/>
-      <c r="I12" s="124"/>
+      <c r="F12" s="97"/>
+      <c r="G12" s="95"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -6161,24 +6255,24 @@
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
-      <c r="X12" s="120"/>
-      <c r="Y12" s="121"/>
-      <c r="Z12" s="121"/>
-      <c r="AA12" s="121"/>
-      <c r="AB12" s="122"/>
-      <c r="AC12" s="122"/>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="93"/>
+      <c r="Z12" s="93"/>
+      <c r="AA12" s="93"/>
+      <c r="AB12" s="94"/>
+      <c r="AC12" s="94"/>
     </row>
     <row r="13" spans="2:29" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="127" t="s">
-        <v>125</v>
-      </c>
-      <c r="C13" s="127"/>
-      <c r="D13" s="127"/>
-      <c r="E13" s="127"/>
-      <c r="F13" s="132"/>
-      <c r="G13" s="124"/>
-      <c r="H13" s="124"/>
-      <c r="I13" s="124"/>
+      <c r="B13" s="131" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="131"/>
+      <c r="D13" s="131"/>
+      <c r="E13" s="131"/>
+      <c r="F13" s="97"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
@@ -6191,13 +6285,13 @@
     </row>
     <row r="14" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B14" s="3"/>
-      <c r="C14" s="138"/>
-      <c r="D14" s="138"/>
-      <c r="E14" s="138"/>
-      <c r="F14" s="138"/>
-      <c r="G14" s="124"/>
-      <c r="H14" s="124"/>
-      <c r="I14" s="124"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -6210,13 +6304,13 @@
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B15" s="3"/>
-      <c r="C15" s="124"/>
-      <c r="D15" s="124"/>
-      <c r="E15" s="124"/>
-      <c r="F15" s="124"/>
-      <c r="G15" s="124"/>
-      <c r="H15" s="124"/>
-      <c r="I15" s="124"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
@@ -6229,15 +6323,15 @@
     </row>
     <row r="16" spans="2:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C16" s="123"/>
-      <c r="D16" s="124"/>
-      <c r="E16" s="124"/>
-      <c r="F16" s="124"/>
-      <c r="G16" s="124"/>
-      <c r="H16" s="124"/>
-      <c r="I16" s="124"/>
+        <v>102</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
@@ -6249,22 +6343,22 @@
       <c r="R16" s="3"/>
     </row>
     <row r="17" spans="2:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="156" t="s">
-        <v>102</v>
-      </c>
-      <c r="C17" s="148" t="s">
+      <c r="B17" s="132" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="149" t="s">
+      <c r="D17" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="149"/>
-      <c r="F17" s="149" t="s">
+      <c r="E17" s="133"/>
+      <c r="F17" s="133" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="149"/>
-      <c r="H17" s="139"/>
-      <c r="I17" s="128"/>
+      <c r="G17" s="133"/>
+      <c r="H17" s="101"/>
+      <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -6276,24 +6370,24 @@
       <c r="R17" s="3"/>
     </row>
     <row r="18" spans="2:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="156"/>
-      <c r="C18" s="150" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="150" t="s">
+      <c r="B18" s="132"/>
+      <c r="C18" s="111" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="111" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="150" t="s">
+      <c r="E18" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="150" t="s">
+      <c r="F18" s="111" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="150" t="s">
+      <c r="G18" s="111" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="133"/>
-      <c r="I18" s="129"/>
+      <c r="H18" s="98"/>
+      <c r="I18" s="32"/>
       <c r="J18" s="32"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
@@ -6305,31 +6399,31 @@
       <c r="R18" s="3"/>
     </row>
     <row r="19" spans="2:18" ht="32" x14ac:dyDescent="0.2">
-      <c r="B19" s="153" t="s">
-        <v>126</v>
-      </c>
-      <c r="C19" s="153">
+      <c r="B19" s="114" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" s="114">
         <f>C9*C10</f>
         <v>1800000</v>
       </c>
-      <c r="D19" s="154">
+      <c r="D19" s="115">
         <f>C9-(D10*C9)</f>
         <v>2160000</v>
       </c>
-      <c r="E19" s="152">
+      <c r="E19" s="113">
         <f>C9-(E10*C9)</f>
         <v>1440000</v>
       </c>
-      <c r="F19" s="152">
+      <c r="F19" s="113">
         <f>C9-(E10*C9)</f>
         <v>1440000</v>
       </c>
-      <c r="G19" s="152">
+      <c r="G19" s="113">
         <f>C9-(D10*C9)</f>
         <v>2160000</v>
       </c>
       <c r="H19" s="49"/>
-      <c r="I19" s="130"/>
+      <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
@@ -6342,30 +6436,30 @@
     </row>
     <row r="20" spans="2:18" ht="32" x14ac:dyDescent="0.2">
       <c r="B20" s="57" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C20" s="57">
         <f>C19*C11</f>
         <v>18000</v>
       </c>
-      <c r="D20" s="155">
+      <c r="D20" s="116">
         <f>C19*D11</f>
         <v>9000</v>
       </c>
-      <c r="E20" s="140">
+      <c r="E20" s="102">
         <f>C19*E11</f>
         <v>36000</v>
       </c>
-      <c r="F20" s="140">
+      <c r="F20" s="102">
         <f>F19*D11</f>
         <v>7200</v>
       </c>
-      <c r="G20" s="140">
+      <c r="G20" s="102">
         <f>G19*E11</f>
         <v>43200</v>
       </c>
       <c r="H20" s="49"/>
-      <c r="I20" s="130"/>
+      <c r="I20" s="18"/>
       <c r="J20" s="18"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
@@ -6378,30 +6472,30 @@
     </row>
     <row r="21" spans="2:18" ht="32" x14ac:dyDescent="0.2">
       <c r="B21" s="57" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C21" s="57">
         <f>C20*C12</f>
         <v>1350</v>
       </c>
-      <c r="D21" s="155">
+      <c r="D21" s="116">
         <f>C20*D12</f>
         <v>900</v>
       </c>
-      <c r="E21" s="140">
+      <c r="E21" s="102">
         <f>C20*E12</f>
         <v>1800</v>
       </c>
-      <c r="F21" s="140">
+      <c r="F21" s="102">
         <f>F20*D12</f>
         <v>360</v>
       </c>
-      <c r="G21" s="140">
+      <c r="G21" s="102">
         <f>G20*E12</f>
         <v>4320</v>
       </c>
       <c r="H21" s="49"/>
-      <c r="I21" s="130"/>
+      <c r="I21" s="18"/>
       <c r="J21" s="18"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
@@ -6414,7 +6508,7 @@
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B22" s="41" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="41"/>
       <c r="D22" s="3"/>
@@ -6422,7 +6516,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="49"/>
-      <c r="I22" s="130"/>
+      <c r="I22" s="18"/>
       <c r="J22" s="18"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
@@ -6435,7 +6529,7 @@
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B23" s="41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="41"/>
       <c r="D23" s="40"/>
@@ -6455,14 +6549,14 @@
       <c r="R23" s="3"/>
     </row>
     <row r="24" spans="2:18" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="97"/>
-      <c r="D24" s="97"/>
-      <c r="E24" s="97"/>
-      <c r="F24" s="97"/>
-      <c r="G24" s="97"/>
+      <c r="B24" s="134" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="134"/>
+      <c r="D24" s="134"/>
+      <c r="E24" s="134"/>
+      <c r="F24" s="134"/>
+      <c r="G24" s="134"/>
       <c r="H24" s="40"/>
       <c r="I24" s="40"/>
       <c r="J24" s="3"/>
@@ -6476,24 +6570,24 @@
       <c r="R24" s="3"/>
     </row>
     <row r="25" spans="2:18" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="97" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="97"/>
-      <c r="D25" s="97"/>
-      <c r="E25" s="97"/>
-      <c r="F25" s="97"/>
-      <c r="G25" s="97"/>
+      <c r="B25" s="134" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="134"/>
+      <c r="D25" s="134"/>
+      <c r="E25" s="134"/>
+      <c r="F25" s="134"/>
+      <c r="G25" s="134"/>
       <c r="H25" s="40"/>
       <c r="I25" s="46"/>
-      <c r="J25" s="134"/>
-      <c r="K25" s="134"/>
-      <c r="L25" s="134"/>
-      <c r="M25" s="134"/>
-      <c r="N25" s="134"/>
-      <c r="O25" s="134"/>
-      <c r="P25" s="134"/>
-      <c r="Q25" s="134"/>
+      <c r="J25" s="99"/>
+      <c r="K25" s="99"/>
+      <c r="L25" s="99"/>
+      <c r="M25" s="99"/>
+      <c r="N25" s="99"/>
+      <c r="O25" s="99"/>
+      <c r="P25" s="99"/>
+      <c r="Q25" s="99"/>
       <c r="R25" s="3"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.2">
@@ -6505,14 +6599,14 @@
       <c r="G26" s="40"/>
       <c r="H26" s="40"/>
       <c r="I26" s="46"/>
-      <c r="J26" s="134"/>
-      <c r="K26" s="134"/>
-      <c r="L26" s="134"/>
-      <c r="M26" s="134"/>
-      <c r="N26" s="134"/>
-      <c r="O26" s="134"/>
-      <c r="P26" s="134"/>
-      <c r="Q26" s="134"/>
+      <c r="J26" s="99"/>
+      <c r="K26" s="99"/>
+      <c r="L26" s="99"/>
+      <c r="M26" s="99"/>
+      <c r="N26" s="99"/>
+      <c r="O26" s="99"/>
+      <c r="P26" s="99"/>
+      <c r="Q26" s="99"/>
       <c r="R26" s="3"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.2">
@@ -6708,15 +6802,15 @@
       <c r="R36" s="3"/>
     </row>
     <row r="37" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" s="96"/>
-      <c r="D37" s="96"/>
-      <c r="E37" s="96"/>
-      <c r="F37" s="96"/>
-      <c r="G37" s="96"/>
-      <c r="H37" s="135"/>
+      <c r="B37" s="129" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="129"/>
+      <c r="D37" s="129"/>
+      <c r="E37" s="129"/>
+      <c r="F37" s="129"/>
+      <c r="G37" s="129"/>
+      <c r="H37" s="3"/>
       <c r="I37" s="38"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
@@ -6729,14 +6823,14 @@
       <c r="R37" s="3"/>
     </row>
     <row r="38" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B38" s="94" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38" s="94"/>
-      <c r="D38" s="94"/>
-      <c r="E38" s="94"/>
-      <c r="F38" s="94"/>
-      <c r="G38" s="94"/>
+      <c r="B38" s="128" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="128"/>
+      <c r="D38" s="128"/>
+      <c r="E38" s="128"/>
+      <c r="F38" s="128"/>
+      <c r="G38" s="128"/>
       <c r="H38" s="35"/>
       <c r="I38" s="36"/>
       <c r="J38" s="3"/>
@@ -6750,14 +6844,14 @@
       <c r="R38" s="3"/>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B39" s="94" t="s">
-        <v>31</v>
-      </c>
-      <c r="C39" s="94"/>
-      <c r="D39" s="94"/>
-      <c r="E39" s="94"/>
-      <c r="F39" s="94"/>
-      <c r="G39" s="94"/>
+      <c r="B39" s="128" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="128"/>
+      <c r="D39" s="128"/>
+      <c r="E39" s="128"/>
+      <c r="F39" s="128"/>
+      <c r="G39" s="128"/>
       <c r="H39" s="35"/>
       <c r="I39" s="36"/>
       <c r="J39" s="3"/>
@@ -6771,14 +6865,14 @@
       <c r="R39" s="3"/>
     </row>
     <row r="40" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="94" t="s">
-        <v>32</v>
-      </c>
-      <c r="C40" s="94"/>
-      <c r="D40" s="94"/>
-      <c r="E40" s="94"/>
-      <c r="F40" s="94"/>
-      <c r="G40" s="94"/>
+      <c r="B40" s="128" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="128"/>
+      <c r="D40" s="128"/>
+      <c r="E40" s="128"/>
+      <c r="F40" s="128"/>
+      <c r="G40" s="128"/>
       <c r="H40" s="35"/>
       <c r="I40" s="36"/>
       <c r="J40" s="3"/>
@@ -6792,14 +6886,14 @@
       <c r="R40" s="3"/>
     </row>
     <row r="41" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="94" t="s">
-        <v>33</v>
-      </c>
-      <c r="C41" s="94"/>
-      <c r="D41" s="94"/>
-      <c r="E41" s="94"/>
-      <c r="F41" s="94"/>
-      <c r="G41" s="94"/>
+      <c r="B41" s="128" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="128"/>
+      <c r="D41" s="128"/>
+      <c r="E41" s="128"/>
+      <c r="F41" s="128"/>
+      <c r="G41" s="128"/>
       <c r="H41" s="35"/>
       <c r="I41" s="36"/>
       <c r="J41" s="3"/>
@@ -6833,17 +6927,17 @@
     </row>
     <row r="44" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B44" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B45" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B46" s="44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C46" s="45" t="s">
         <v>14</v>
@@ -6863,7 +6957,7 @@
     </row>
     <row r="47" spans="2:18" ht="48" x14ac:dyDescent="0.2">
       <c r="B47" s="42" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C47" s="43">
         <f>F47-E47</f>
@@ -6888,7 +6982,7 @@
     </row>
     <row r="48" spans="2:18" ht="48" x14ac:dyDescent="0.2">
       <c r="B48" s="42" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C48" s="43">
         <f>F48-E48</f>
@@ -6913,7 +7007,7 @@
     </row>
     <row r="49" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B49" s="42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C49" s="43">
         <f>F49-E49</f>
@@ -6938,19 +7032,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="I8:P10"/>
+    <mergeCell ref="B4:G5"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
     <mergeCell ref="B38:G38"/>
     <mergeCell ref="B37:G37"/>
     <mergeCell ref="B39:G39"/>
     <mergeCell ref="B40:G40"/>
     <mergeCell ref="B41:G41"/>
-    <mergeCell ref="B4:G5"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="I8:P10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6961,8 +7055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A54D747-3B89-BC41-8182-1F289A700DB3}">
   <dimension ref="B1:AH128"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7004,81 +7098,81 @@
       <c r="F2" s="7"/>
     </row>
     <row r="3" spans="2:34" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="105" t="s">
-        <v>133</v>
-      </c>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="105"/>
-      <c r="I3" s="105"/>
-      <c r="J3" s="105"/>
-      <c r="K3" s="105"/>
-      <c r="L3" s="105"/>
-      <c r="M3" s="105"/>
-      <c r="N3" s="105"/>
-      <c r="O3" s="105"/>
-      <c r="P3" s="105"/>
-      <c r="Q3" s="105"/>
-      <c r="R3" s="105"/>
-      <c r="S3" s="105"/>
+      <c r="C3" s="143" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="143"/>
+      <c r="E3" s="143"/>
+      <c r="F3" s="143"/>
+      <c r="G3" s="143"/>
+      <c r="H3" s="143"/>
+      <c r="I3" s="143"/>
+      <c r="J3" s="143"/>
+      <c r="K3" s="143"/>
+      <c r="L3" s="143"/>
+      <c r="M3" s="143"/>
+      <c r="N3" s="143"/>
+      <c r="O3" s="143"/>
+      <c r="P3" s="143"/>
+      <c r="Q3" s="143"/>
+      <c r="R3" s="143"/>
+      <c r="S3" s="143"/>
     </row>
     <row r="6" spans="2:34" ht="26.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="106" t="str">
+      <c r="I6" s="144" t="str">
         <f>_xlfn.CONCAT("Figure 1. Estimated Number of Severe Fetal Outcomes Under Potential Immunity and Infection Rate Scenarios, based on ",D8," Pregnancies")</f>
         <v>Figure 1. Estimated Number of Severe Fetal Outcomes Under Potential Immunity and Infection Rate Scenarios, based on 3600000 Pregnancies</v>
       </c>
-      <c r="J6" s="106"/>
-      <c r="K6" s="106"/>
-      <c r="L6" s="106"/>
-      <c r="M6" s="106"/>
-      <c r="N6" s="106"/>
-      <c r="O6" s="106"/>
-      <c r="P6" s="106"/>
-      <c r="Q6" s="106"/>
-      <c r="R6" s="106"/>
-      <c r="S6" s="106"/>
+      <c r="J6" s="144"/>
+      <c r="K6" s="144"/>
+      <c r="L6" s="144"/>
+      <c r="M6" s="144"/>
+      <c r="N6" s="144"/>
+      <c r="O6" s="144"/>
+      <c r="P6" s="144"/>
+      <c r="Q6" s="144"/>
+      <c r="R6" s="144"/>
+      <c r="S6" s="144"/>
       <c r="T6" s="3"/>
       <c r="W6" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD6" s="60" t="s">
         <v>23</v>
-      </c>
-      <c r="AD6" s="60" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:34" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
-      <c r="C7" s="158" t="s">
+      <c r="C7" s="118" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="159" t="s">
+      <c r="D7" s="119" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="106"/>
-      <c r="J7" s="106"/>
-      <c r="K7" s="106"/>
-      <c r="L7" s="106"/>
-      <c r="M7" s="106"/>
-      <c r="N7" s="106"/>
-      <c r="O7" s="106"/>
-      <c r="P7" s="106"/>
-      <c r="Q7" s="106"/>
-      <c r="R7" s="106"/>
-      <c r="S7" s="106"/>
+      <c r="I7" s="144"/>
+      <c r="J7" s="144"/>
+      <c r="K7" s="144"/>
+      <c r="L7" s="144"/>
+      <c r="M7" s="144"/>
+      <c r="N7" s="144"/>
+      <c r="O7" s="144"/>
+      <c r="P7" s="144"/>
+      <c r="Q7" s="144"/>
+      <c r="R7" s="144"/>
+      <c r="S7" s="144"/>
       <c r="T7" s="3"/>
       <c r="W7" s="55" t="s">
         <v>4</v>
@@ -7113,16 +7207,16 @@
     </row>
     <row r="8" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
-      <c r="C8" s="151" t="s">
-        <v>39</v>
+      <c r="C8" s="112" t="s">
+        <v>38</v>
       </c>
       <c r="D8" s="47">
         <v>3600000</v>
       </c>
       <c r="E8" s="49"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="100" t="s">
-        <v>139</v>
+      <c r="G8" s="142" t="s">
+        <v>136</v>
       </c>
       <c r="H8" s="13">
         <v>0.75</v>
@@ -7211,15 +7305,15 @@
     </row>
     <row r="9" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
-      <c r="C9" s="141" t="s">
-        <v>134</v>
-      </c>
-      <c r="D9" s="144" t="s">
-        <v>45</v>
+      <c r="C9" s="103" t="s">
+        <v>131</v>
+      </c>
+      <c r="D9" s="106" t="s">
+        <v>44</v>
       </c>
       <c r="E9" s="50"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="100"/>
+      <c r="G9" s="142"/>
       <c r="H9" s="13">
         <v>0.7</v>
       </c>
@@ -7307,15 +7401,15 @@
     </row>
     <row r="10" spans="2:34" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
-      <c r="C10" s="141" t="s">
-        <v>135</v>
-      </c>
-      <c r="D10" s="144" t="s">
+      <c r="C10" s="103" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" s="106" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="50"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="100"/>
+      <c r="G10" s="142"/>
       <c r="H10" s="13">
         <v>0.65</v>
       </c>
@@ -7403,15 +7497,15 @@
     </row>
     <row r="11" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
-      <c r="C11" s="141" t="s">
-        <v>136</v>
-      </c>
-      <c r="D11" s="157">
+      <c r="C11" s="103" t="s">
+        <v>133</v>
+      </c>
+      <c r="D11" s="117">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="E11" s="51"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="100"/>
+      <c r="G11" s="142"/>
       <c r="H11" s="13">
         <v>0.6</v>
       </c>
@@ -7419,15 +7513,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J11" s="18">
+      <c r="J11" s="28">
         <f t="shared" si="2"/>
         <v>1080</v>
       </c>
-      <c r="K11" s="28">
+      <c r="K11" s="29">
         <f t="shared" si="14"/>
         <v>2160</v>
       </c>
-      <c r="L11" s="29">
+      <c r="L11" s="62">
         <f t="shared" si="3"/>
         <v>3240</v>
       </c>
@@ -7439,15 +7533,15 @@
         <f t="shared" si="5"/>
         <v>5400</v>
       </c>
-      <c r="O11" s="18">
+      <c r="O11" s="120">
         <f t="shared" si="6"/>
         <v>6480</v>
       </c>
-      <c r="P11" s="18">
+      <c r="P11" s="121">
         <f t="shared" si="7"/>
         <v>7560.0000000000009</v>
       </c>
-      <c r="Q11" s="18">
+      <c r="Q11" s="122">
         <f t="shared" si="8"/>
         <v>8640</v>
       </c>
@@ -7499,11 +7593,11 @@
     </row>
     <row r="12" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="3"/>
-      <c r="C12" s="125"/>
+      <c r="C12" s="35"/>
       <c r="D12" s="51"/>
       <c r="E12" s="51"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="100"/>
+      <c r="G12" s="142"/>
       <c r="H12" s="13">
         <v>0.55000000000000004</v>
       </c>
@@ -7511,15 +7605,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J12" s="18">
+      <c r="J12" s="62">
         <f t="shared" si="2"/>
         <v>1214.9999999999998</v>
       </c>
-      <c r="K12" s="62">
+      <c r="K12" s="63">
         <f t="shared" si="14"/>
         <v>2429.9999999999995</v>
       </c>
-      <c r="L12" s="63">
+      <c r="L12" s="62">
         <f t="shared" si="3"/>
         <v>3644.9999999999995</v>
       </c>
@@ -7531,7 +7625,7 @@
         <f t="shared" si="5"/>
         <v>6075</v>
       </c>
-      <c r="O12" s="18">
+      <c r="O12" s="123">
         <f t="shared" si="6"/>
         <v>7289.9999999999991</v>
       </c>
@@ -7539,7 +7633,7 @@
         <f t="shared" si="7"/>
         <v>8505</v>
       </c>
-      <c r="Q12" s="18">
+      <c r="Q12" s="124">
         <f t="shared" si="8"/>
         <v>9719.9999999999982</v>
       </c>
@@ -7595,7 +7689,7 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="100"/>
+      <c r="G13" s="142"/>
       <c r="H13" s="13">
         <v>0.5</v>
       </c>
@@ -7603,15 +7697,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J13" s="18">
+      <c r="J13" s="62">
         <f t="shared" si="2"/>
         <v>1350</v>
       </c>
-      <c r="K13" s="62">
+      <c r="K13" s="63">
         <f t="shared" si="14"/>
         <v>2700</v>
       </c>
-      <c r="L13" s="63">
+      <c r="L13" s="62">
         <f t="shared" si="3"/>
         <v>4050</v>
       </c>
@@ -7623,7 +7717,7 @@
         <f t="shared" si="5"/>
         <v>6750</v>
       </c>
-      <c r="O13" s="18">
+      <c r="O13" s="123">
         <f t="shared" si="6"/>
         <v>8100</v>
       </c>
@@ -7631,7 +7725,7 @@
         <f t="shared" si="7"/>
         <v>9450</v>
       </c>
-      <c r="Q13" s="18">
+      <c r="Q13" s="124">
         <f t="shared" si="8"/>
         <v>10800</v>
       </c>
@@ -7689,7 +7783,7 @@
       <c r="D14" s="24"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="100"/>
+      <c r="G14" s="142"/>
       <c r="H14" s="13">
         <v>0.45</v>
       </c>
@@ -7697,15 +7791,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J14" s="18">
+      <c r="J14" s="62">
         <f t="shared" si="2"/>
         <v>1485</v>
       </c>
-      <c r="K14" s="62">
+      <c r="K14" s="63">
         <f t="shared" si="14"/>
         <v>2970</v>
       </c>
-      <c r="L14" s="63">
+      <c r="L14" s="62">
         <f t="shared" si="3"/>
         <v>4455</v>
       </c>
@@ -7717,7 +7811,7 @@
         <f t="shared" si="5"/>
         <v>7425</v>
       </c>
-      <c r="O14" s="18">
+      <c r="O14" s="123">
         <f t="shared" si="6"/>
         <v>8910</v>
       </c>
@@ -7725,7 +7819,7 @@
         <f t="shared" si="7"/>
         <v>10395</v>
       </c>
-      <c r="Q14" s="18">
+      <c r="Q14" s="124">
         <f t="shared" si="8"/>
         <v>11880</v>
       </c>
@@ -7777,13 +7871,13 @@
     </row>
     <row r="15" spans="2:34" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
-      <c r="C15" s="109" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="110"/>
+      <c r="C15" s="145" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="146"/>
       <c r="E15" s="48"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="100"/>
+      <c r="G15" s="142"/>
       <c r="H15" s="13">
         <v>0.4</v>
       </c>
@@ -7791,15 +7885,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J15" s="30">
         <f t="shared" si="2"/>
         <v>1620</v>
       </c>
-      <c r="K15" s="30">
+      <c r="K15" s="31">
         <f t="shared" si="14"/>
         <v>3240</v>
       </c>
-      <c r="L15" s="31">
+      <c r="L15" s="62">
         <f t="shared" si="3"/>
         <v>4860</v>
       </c>
@@ -7811,15 +7905,15 @@
         <f t="shared" si="5"/>
         <v>8100</v>
       </c>
-      <c r="O15" s="18">
+      <c r="O15" s="125">
         <f t="shared" si="6"/>
         <v>9720</v>
       </c>
-      <c r="P15" s="18">
+      <c r="P15" s="126">
         <f t="shared" si="7"/>
         <v>11340</v>
       </c>
-      <c r="Q15" s="18">
+      <c r="Q15" s="127">
         <f t="shared" si="8"/>
         <v>12960</v>
       </c>
@@ -7871,11 +7965,11 @@
     </row>
     <row r="16" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="3"/>
-      <c r="C16" s="111"/>
-      <c r="D16" s="110"/>
+      <c r="C16" s="147"/>
+      <c r="D16" s="146"/>
       <c r="E16" s="48"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="100"/>
+      <c r="G16" s="142"/>
       <c r="H16" s="13">
         <v>0.35</v>
       </c>
@@ -7963,13 +8057,13 @@
     </row>
     <row r="17" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="3"/>
-      <c r="C17" s="107" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="108"/>
+      <c r="C17" s="148" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="149"/>
       <c r="E17" s="36"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="100"/>
+      <c r="G17" s="142"/>
       <c r="H17" s="13">
         <v>0.3</v>
       </c>
@@ -8057,13 +8151,13 @@
     </row>
     <row r="18" spans="2:34" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
-      <c r="C18" s="107" t="s">
-        <v>137</v>
-      </c>
-      <c r="D18" s="108"/>
+      <c r="C18" s="148" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" s="149"/>
       <c r="E18" s="36"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="100"/>
+      <c r="G18" s="142"/>
       <c r="H18" s="13">
         <v>0.25</v>
       </c>
@@ -8151,8 +8245,8 @@
     </row>
     <row r="19" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
-      <c r="C19" s="112"/>
-      <c r="D19" s="108"/>
+      <c r="C19" s="150"/>
+      <c r="D19" s="149"/>
       <c r="E19" s="36"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -8230,25 +8324,25 @@
     </row>
     <row r="20" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B20" s="3"/>
-      <c r="C20" s="112"/>
-      <c r="D20" s="108"/>
+      <c r="C20" s="150"/>
+      <c r="D20" s="149"/>
       <c r="E20" s="36"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="101" t="s">
-        <v>138</v>
-      </c>
-      <c r="J20" s="101"/>
-      <c r="K20" s="101"/>
-      <c r="L20" s="101"/>
-      <c r="M20" s="101"/>
-      <c r="N20" s="101"/>
-      <c r="O20" s="101"/>
-      <c r="P20" s="101"/>
-      <c r="Q20" s="101"/>
-      <c r="R20" s="101"/>
-      <c r="S20" s="101"/>
+      <c r="I20" s="136" t="s">
+        <v>135</v>
+      </c>
+      <c r="J20" s="136"/>
+      <c r="K20" s="136"/>
+      <c r="L20" s="136"/>
+      <c r="M20" s="136"/>
+      <c r="N20" s="136"/>
+      <c r="O20" s="136"/>
+      <c r="P20" s="136"/>
+      <c r="Q20" s="136"/>
+      <c r="R20" s="136"/>
+      <c r="S20" s="136"/>
       <c r="T20" s="3"/>
       <c r="W20" s="56">
         <v>0.01</v>
@@ -8289,14 +8383,14 @@
     </row>
     <row r="21" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B21" s="3"/>
-      <c r="C21" s="112"/>
-      <c r="D21" s="108"/>
+      <c r="C21" s="150"/>
+      <c r="D21" s="149"/>
       <c r="E21" s="36"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -8348,13 +8442,15 @@
     </row>
     <row r="22" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
-      <c r="C22" s="113"/>
-      <c r="D22" s="114"/>
+      <c r="C22" s="151"/>
+      <c r="D22" s="152"/>
       <c r="E22" s="36"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
+      <c r="I22" s="3" t="s">
+        <v>145</v>
+      </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
@@ -8527,20 +8623,20 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
-      <c r="I25" s="102" t="str">
+      <c r="I25" s="139" t="str">
         <f>_xlfn.CONCAT("Figure 2. Estimated Number of Severe Fetal Outcomes Under all Possible Immunity and Infection Rate Scenarios, based on ",D8," Pregnancies")</f>
         <v>Figure 2. Estimated Number of Severe Fetal Outcomes Under all Possible Immunity and Infection Rate Scenarios, based on 3600000 Pregnancies</v>
       </c>
-      <c r="J25" s="102"/>
-      <c r="K25" s="102"/>
-      <c r="L25" s="102"/>
-      <c r="M25" s="102"/>
-      <c r="N25" s="102"/>
-      <c r="O25" s="102"/>
-      <c r="P25" s="102"/>
-      <c r="Q25" s="102"/>
-      <c r="R25" s="102"/>
-      <c r="S25" s="102"/>
+      <c r="J25" s="139"/>
+      <c r="K25" s="139"/>
+      <c r="L25" s="139"/>
+      <c r="M25" s="139"/>
+      <c r="N25" s="139"/>
+      <c r="O25" s="139"/>
+      <c r="P25" s="139"/>
+      <c r="Q25" s="139"/>
+      <c r="R25" s="139"/>
+      <c r="S25" s="139"/>
       <c r="T25" s="3"/>
       <c r="W25" s="56">
         <v>0.01</v>
@@ -8581,25 +8677,25 @@
     </row>
     <row r="26" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="3"/>
-      <c r="C26" s="104" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="104"/>
+      <c r="C26" s="141" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="141"/>
       <c r="E26" s="48"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
-      <c r="I26" s="103"/>
-      <c r="J26" s="103"/>
-      <c r="K26" s="103"/>
-      <c r="L26" s="103"/>
-      <c r="M26" s="103"/>
-      <c r="N26" s="103"/>
-      <c r="O26" s="103"/>
-      <c r="P26" s="103"/>
-      <c r="Q26" s="103"/>
-      <c r="R26" s="103"/>
-      <c r="S26" s="103"/>
+      <c r="I26" s="140"/>
+      <c r="J26" s="140"/>
+      <c r="K26" s="140"/>
+      <c r="L26" s="140"/>
+      <c r="M26" s="140"/>
+      <c r="N26" s="140"/>
+      <c r="O26" s="140"/>
+      <c r="P26" s="140"/>
+      <c r="Q26" s="140"/>
+      <c r="R26" s="140"/>
+      <c r="S26" s="140"/>
       <c r="T26" s="3"/>
       <c r="W26" s="56">
         <v>0.01</v>
@@ -8640,12 +8736,12 @@
     </row>
     <row r="27" spans="2:34" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="3"/>
-      <c r="C27" s="104"/>
-      <c r="D27" s="104"/>
+      <c r="C27" s="141"/>
+      <c r="D27" s="141"/>
       <c r="E27" s="48"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="100" t="s">
-        <v>139</v>
+      <c r="G27" s="142" t="s">
+        <v>136</v>
       </c>
       <c r="H27" s="13">
         <v>1</v>
@@ -8734,11 +8830,11 @@
     </row>
     <row r="28" spans="2:34" s="8" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="3"/>
-      <c r="C28" s="104"/>
-      <c r="D28" s="104"/>
+      <c r="C28" s="141"/>
+      <c r="D28" s="141"/>
       <c r="E28" s="48"/>
       <c r="F28" s="35"/>
-      <c r="G28" s="100"/>
+      <c r="G28" s="142"/>
       <c r="H28" s="13">
         <v>0.9</v>
       </c>
@@ -8826,13 +8922,13 @@
     </row>
     <row r="29" spans="2:34" s="8" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="3"/>
-      <c r="C29" s="104" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="104"/>
+      <c r="C29" s="141" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="141"/>
       <c r="E29" s="48"/>
       <c r="F29" s="35"/>
-      <c r="G29" s="100"/>
+      <c r="G29" s="142"/>
       <c r="H29" s="13">
         <v>0.8</v>
       </c>
@@ -8918,13 +9014,13 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="30" spans="2:34" s="8" customFormat="1" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:34" s="8" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="35"/>
-      <c r="C30" s="104"/>
-      <c r="D30" s="104"/>
+      <c r="C30" s="141"/>
+      <c r="D30" s="141"/>
       <c r="E30" s="48"/>
       <c r="F30" s="35"/>
-      <c r="G30" s="100"/>
+      <c r="G30" s="142"/>
       <c r="H30" s="13">
         <v>0.7</v>
       </c>
@@ -9012,21 +9108,21 @@
     </row>
     <row r="31" spans="2:34" s="8" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="3"/>
-      <c r="C31" s="104" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31" s="104"/>
+      <c r="C31" s="141" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="141"/>
       <c r="E31" s="48"/>
       <c r="F31" s="35"/>
-      <c r="G31" s="100"/>
+      <c r="G31" s="142"/>
       <c r="H31" s="13">
         <v>0.6</v>
       </c>
-      <c r="I31" s="28">
+      <c r="I31" s="17">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="J31" s="29">
+      <c r="J31" s="18">
         <f t="shared" si="19"/>
         <v>10800</v>
       </c>
@@ -9106,19 +9202,19 @@
     </row>
     <row r="32" spans="2:34" s="8" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="35"/>
-      <c r="C32" s="104"/>
-      <c r="D32" s="104"/>
+      <c r="C32" s="141"/>
+      <c r="D32" s="141"/>
       <c r="E32" s="48"/>
       <c r="F32" s="35"/>
-      <c r="G32" s="100"/>
+      <c r="G32" s="142"/>
       <c r="H32" s="13">
         <v>0.5</v>
       </c>
-      <c r="I32" s="62">
+      <c r="I32" s="17">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="J32" s="63">
+      <c r="J32" s="18">
         <f t="shared" si="19"/>
         <v>13500</v>
       </c>
@@ -9196,23 +9292,23 @@
         <v>10800</v>
       </c>
     </row>
-    <row r="33" spans="2:34" s="8" customFormat="1" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:34" s="8" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="35"/>
-      <c r="C33" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="D33" s="104"/>
+      <c r="C33" s="141" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="141"/>
       <c r="E33" s="48"/>
       <c r="F33" s="35"/>
-      <c r="G33" s="100"/>
+      <c r="G33" s="142"/>
       <c r="H33" s="13">
         <v>0.4</v>
       </c>
-      <c r="I33" s="30">
+      <c r="I33" s="17">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="J33" s="31">
+      <c r="J33" s="18">
         <f t="shared" si="19"/>
         <v>16200</v>
       </c>
@@ -9292,11 +9388,11 @@
     </row>
     <row r="34" spans="2:34" s="8" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="35"/>
-      <c r="C34" s="104"/>
-      <c r="D34" s="104"/>
+      <c r="C34" s="141"/>
+      <c r="D34" s="141"/>
       <c r="E34" s="48"/>
       <c r="F34" s="35"/>
-      <c r="G34" s="100"/>
+      <c r="G34" s="142"/>
       <c r="H34" s="13">
         <v>0.3</v>
       </c>
@@ -9384,13 +9480,13 @@
     </row>
     <row r="35" spans="2:34" s="8" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="35"/>
-      <c r="C35" s="104" t="s">
-        <v>28</v>
-      </c>
-      <c r="D35" s="104"/>
+      <c r="C35" s="141" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="141"/>
       <c r="E35" s="48"/>
       <c r="F35" s="35"/>
-      <c r="G35" s="100"/>
+      <c r="G35" s="142"/>
       <c r="H35" s="13">
         <v>0.2</v>
       </c>
@@ -9478,11 +9574,11 @@
     </row>
     <row r="36" spans="2:34" s="8" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="35"/>
-      <c r="C36" s="104"/>
-      <c r="D36" s="104"/>
+      <c r="C36" s="141"/>
+      <c r="D36" s="141"/>
       <c r="E36" s="48"/>
       <c r="F36" s="35"/>
-      <c r="G36" s="100"/>
+      <c r="G36" s="142"/>
       <c r="H36" s="13">
         <v>0.1</v>
       </c>
@@ -9574,7 +9670,7 @@
       <c r="D37" s="35"/>
       <c r="E37" s="35"/>
       <c r="F37" s="35"/>
-      <c r="G37" s="100"/>
+      <c r="G37" s="142"/>
       <c r="H37" s="13">
         <v>0</v>
       </c>
@@ -9747,19 +9843,19 @@
       <c r="F39" s="35"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
-      <c r="I39" s="101" t="s">
-        <v>138</v>
-      </c>
-      <c r="J39" s="101"/>
-      <c r="K39" s="101"/>
-      <c r="L39" s="101"/>
-      <c r="M39" s="101"/>
-      <c r="N39" s="101"/>
-      <c r="O39" s="101"/>
-      <c r="P39" s="101"/>
-      <c r="Q39" s="101"/>
-      <c r="R39" s="101"/>
-      <c r="S39" s="101"/>
+      <c r="I39" s="136" t="s">
+        <v>135</v>
+      </c>
+      <c r="J39" s="136"/>
+      <c r="K39" s="136"/>
+      <c r="L39" s="136"/>
+      <c r="M39" s="136"/>
+      <c r="N39" s="136"/>
+      <c r="O39" s="136"/>
+      <c r="P39" s="136"/>
+      <c r="Q39" s="136"/>
+      <c r="R39" s="136"/>
+      <c r="S39" s="136"/>
       <c r="T39" s="3"/>
       <c r="W39" s="56">
         <v>0.02</v>
@@ -9863,9 +9959,7 @@
       <c r="F41" s="35"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
-      <c r="I41" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
@@ -10926,7 +11020,7 @@
       </c>
     </row>
     <row r="68" spans="14:34" x14ac:dyDescent="0.2">
-      <c r="N68" s="99"/>
+      <c r="N68" s="137"/>
       <c r="O68" s="10"/>
       <c r="P68" s="11"/>
       <c r="Q68" s="11"/>
@@ -10971,7 +11065,7 @@
       </c>
     </row>
     <row r="69" spans="14:34" x14ac:dyDescent="0.2">
-      <c r="N69" s="99"/>
+      <c r="N69" s="137"/>
       <c r="O69" s="10"/>
       <c r="P69" s="11"/>
       <c r="Q69" s="11"/>
@@ -11016,7 +11110,7 @@
       </c>
     </row>
     <row r="70" spans="14:34" x14ac:dyDescent="0.2">
-      <c r="N70" s="99"/>
+      <c r="N70" s="137"/>
       <c r="O70" s="10"/>
       <c r="P70" s="11"/>
       <c r="Q70" s="11"/>
@@ -11061,7 +11155,7 @@
       </c>
     </row>
     <row r="71" spans="14:34" x14ac:dyDescent="0.2">
-      <c r="N71" s="99"/>
+      <c r="N71" s="137"/>
       <c r="O71" s="10"/>
       <c r="P71" s="11"/>
       <c r="Q71" s="11"/>
@@ -11106,7 +11200,7 @@
       </c>
     </row>
     <row r="72" spans="14:34" x14ac:dyDescent="0.2">
-      <c r="N72" s="99"/>
+      <c r="N72" s="137"/>
       <c r="O72" s="10"/>
       <c r="P72" s="11"/>
       <c r="Q72" s="11"/>
@@ -11194,11 +11288,11 @@
       </c>
     </row>
     <row r="74" spans="14:34" x14ac:dyDescent="0.2">
-      <c r="P74" s="98"/>
-      <c r="Q74" s="98"/>
-      <c r="R74" s="98"/>
-      <c r="S74" s="98"/>
-      <c r="T74" s="98"/>
+      <c r="P74" s="138"/>
+      <c r="Q74" s="138"/>
+      <c r="R74" s="138"/>
+      <c r="S74" s="138"/>
+      <c r="T74" s="138"/>
       <c r="W74" s="56">
         <v>0.06</v>
       </c>
@@ -13290,6 +13384,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C3:S3"/>
+    <mergeCell ref="I6:S7"/>
+    <mergeCell ref="G8:G18"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D22"/>
+    <mergeCell ref="I20:S20"/>
     <mergeCell ref="I39:S39"/>
     <mergeCell ref="N68:N72"/>
     <mergeCell ref="P74:T74"/>
@@ -13300,13 +13401,6 @@
     <mergeCell ref="C31:D32"/>
     <mergeCell ref="C33:D34"/>
     <mergeCell ref="C35:D36"/>
-    <mergeCell ref="C3:S3"/>
-    <mergeCell ref="I6:S7"/>
-    <mergeCell ref="G8:G18"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D22"/>
-    <mergeCell ref="I20:S20"/>
   </mergeCells>
   <conditionalFormatting sqref="I8:S18">
     <cfRule type="colorScale" priority="1">
@@ -13375,20 +13469,20 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:13" ht="19" x14ac:dyDescent="0.25">
-      <c r="B4" s="115" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
-      <c r="H4" s="115"/>
-      <c r="I4" s="115"/>
-      <c r="J4" s="115"/>
-      <c r="K4" s="115"/>
-      <c r="L4" s="115"/>
-      <c r="M4" s="115"/>
+      <c r="B4" s="153" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="153"/>
+      <c r="D4" s="153"/>
+      <c r="E4" s="153"/>
+      <c r="F4" s="153"/>
+      <c r="G4" s="153"/>
+      <c r="H4" s="153"/>
+      <c r="I4" s="153"/>
+      <c r="J4" s="153"/>
+      <c r="K4" s="153"/>
+      <c r="L4" s="153"/>
+      <c r="M4" s="153"/>
     </row>
     <row r="5" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="70"/>
@@ -13407,7 +13501,7 @@
     <row r="6" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
       <c r="C6" s="65" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -13423,7 +13517,7 @@
     <row r="7" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="3"/>
       <c r="C7" s="65" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -13439,7 +13533,7 @@
     <row r="8" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="65" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -13455,7 +13549,7 @@
     <row r="9" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
       <c r="C9" s="65" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -13471,7 +13565,7 @@
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
       <c r="C10" s="66" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -13486,24 +13580,24 @@
     </row>
     <row r="11" spans="2:13" ht="63.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
-      <c r="C11" s="116" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="116"/>
-      <c r="E11" s="116"/>
-      <c r="F11" s="116"/>
-      <c r="G11" s="116"/>
-      <c r="H11" s="116"/>
-      <c r="I11" s="116"/>
-      <c r="J11" s="116"/>
-      <c r="K11" s="116"/>
-      <c r="L11" s="116"/>
+      <c r="C11" s="154" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="154"/>
+      <c r="E11" s="154"/>
+      <c r="F11" s="154"/>
+      <c r="G11" s="154"/>
+      <c r="H11" s="154"/>
+      <c r="I11" s="154"/>
+      <c r="J11" s="154"/>
+      <c r="K11" s="154"/>
+      <c r="L11" s="154"/>
       <c r="M11" s="3"/>
     </row>
     <row r="12" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="3"/>
       <c r="C12" s="65" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -13519,7 +13613,7 @@
     <row r="13" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="3"/>
       <c r="C13" s="67" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -13535,7 +13629,7 @@
     <row r="14" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="3"/>
       <c r="C14" s="67" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -13551,7 +13645,7 @@
     <row r="15" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="3"/>
       <c r="C15" s="67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -13567,7 +13661,7 @@
     <row r="16" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" s="3"/>
       <c r="C16" s="67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -13611,7 +13705,7 @@
     <row r="19" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
       <c r="C19" s="65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -13627,7 +13721,7 @@
     <row r="20" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" s="3"/>
       <c r="C20" s="65" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -13643,7 +13737,7 @@
     <row r="21" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="3"/>
       <c r="C21" s="65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -13659,7 +13753,7 @@
     <row r="22" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" s="3"/>
       <c r="C22" s="65" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -13675,7 +13769,7 @@
     <row r="23" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B23" s="3"/>
       <c r="C23" s="66" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -13690,24 +13784,24 @@
     </row>
     <row r="24" spans="2:13" ht="60.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="3"/>
-      <c r="C24" s="116" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="116"/>
-      <c r="E24" s="116"/>
-      <c r="F24" s="116"/>
-      <c r="G24" s="116"/>
-      <c r="H24" s="116"/>
-      <c r="I24" s="116"/>
-      <c r="J24" s="116"/>
-      <c r="K24" s="116"/>
-      <c r="L24" s="116"/>
+      <c r="C24" s="154" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="154"/>
+      <c r="E24" s="154"/>
+      <c r="F24" s="154"/>
+      <c r="G24" s="154"/>
+      <c r="H24" s="154"/>
+      <c r="I24" s="154"/>
+      <c r="J24" s="154"/>
+      <c r="K24" s="154"/>
+      <c r="L24" s="154"/>
       <c r="M24" s="3"/>
     </row>
     <row r="25" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" s="3"/>
       <c r="C25" s="65" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -13723,7 +13817,7 @@
     <row r="26" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B26" s="3"/>
       <c r="C26" s="67" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -13739,7 +13833,7 @@
     <row r="27" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B27" s="3"/>
       <c r="C27" s="67" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -13783,7 +13877,7 @@
     <row r="30" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B30" s="3"/>
       <c r="C30" s="65" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -13799,7 +13893,7 @@
     <row r="31" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B31" s="3"/>
       <c r="C31" s="65" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -13815,7 +13909,7 @@
     <row r="32" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B32" s="3"/>
       <c r="C32" s="65" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -13831,7 +13925,7 @@
     <row r="33" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B33" s="3"/>
       <c r="C33" s="65" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -13847,7 +13941,7 @@
     <row r="34" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B34" s="3"/>
       <c r="C34" s="66" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
@@ -13862,24 +13956,24 @@
     </row>
     <row r="35" spans="2:13" ht="51.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="3"/>
-      <c r="C35" s="116" t="s">
-        <v>75</v>
-      </c>
-      <c r="D35" s="116"/>
-      <c r="E35" s="116"/>
-      <c r="F35" s="116"/>
-      <c r="G35" s="116"/>
-      <c r="H35" s="116"/>
-      <c r="I35" s="116"/>
-      <c r="J35" s="116"/>
-      <c r="K35" s="116"/>
-      <c r="L35" s="116"/>
+      <c r="C35" s="154" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" s="154"/>
+      <c r="E35" s="154"/>
+      <c r="F35" s="154"/>
+      <c r="G35" s="154"/>
+      <c r="H35" s="154"/>
+      <c r="I35" s="154"/>
+      <c r="J35" s="154"/>
+      <c r="K35" s="154"/>
+      <c r="L35" s="154"/>
       <c r="M35" s="3"/>
     </row>
     <row r="36" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B36" s="3"/>
       <c r="C36" s="65" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
@@ -13895,7 +13989,7 @@
     <row r="37" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B37" s="3"/>
       <c r="C37" s="67" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
@@ -13911,7 +14005,7 @@
     <row r="38" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B38" s="3"/>
       <c r="C38" s="67" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
@@ -13955,7 +14049,7 @@
     <row r="41" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" s="3"/>
       <c r="C41" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
@@ -13971,7 +14065,7 @@
     <row r="42" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B42" s="3"/>
       <c r="C42" s="65" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
@@ -13987,7 +14081,7 @@
     <row r="43" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B43" s="3"/>
       <c r="C43" s="65" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
@@ -14003,7 +14097,7 @@
     <row r="44" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B44" s="3"/>
       <c r="C44" s="65" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
@@ -14019,7 +14113,7 @@
     <row r="45" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B45" s="3"/>
       <c r="C45" s="66" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
@@ -14034,24 +14128,24 @@
     </row>
     <row r="46" spans="2:13" ht="54.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="3"/>
-      <c r="C46" s="116" t="s">
-        <v>82</v>
-      </c>
-      <c r="D46" s="116"/>
-      <c r="E46" s="116"/>
-      <c r="F46" s="116"/>
-      <c r="G46" s="116"/>
-      <c r="H46" s="116"/>
-      <c r="I46" s="116"/>
-      <c r="J46" s="116"/>
-      <c r="K46" s="116"/>
-      <c r="L46" s="116"/>
+      <c r="C46" s="154" t="s">
+        <v>81</v>
+      </c>
+      <c r="D46" s="154"/>
+      <c r="E46" s="154"/>
+      <c r="F46" s="154"/>
+      <c r="G46" s="154"/>
+      <c r="H46" s="154"/>
+      <c r="I46" s="154"/>
+      <c r="J46" s="154"/>
+      <c r="K46" s="154"/>
+      <c r="L46" s="154"/>
       <c r="M46" s="3"/>
     </row>
     <row r="47" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B47" s="3"/>
       <c r="C47" s="65" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
@@ -14067,7 +14161,7 @@
     <row r="48" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B48" s="3"/>
       <c r="C48" s="67" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D48" s="68"/>
       <c r="E48" s="68"/>
@@ -14083,7 +14177,7 @@
     <row r="49" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B49" s="3"/>
       <c r="C49" s="67" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
@@ -14127,7 +14221,7 @@
     <row r="52" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B52" s="3"/>
       <c r="C52" s="65" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
@@ -14143,7 +14237,7 @@
     <row r="53" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B53" s="3"/>
       <c r="C53" s="65" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
@@ -14159,7 +14253,7 @@
     <row r="54" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B54" s="3"/>
       <c r="C54" s="65" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
@@ -14175,7 +14269,7 @@
     <row r="55" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B55" s="3"/>
       <c r="C55" s="65" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
@@ -14191,7 +14285,7 @@
     <row r="56" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B56" s="3"/>
       <c r="C56" s="66" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
@@ -14206,24 +14300,24 @@
     </row>
     <row r="57" spans="2:13" ht="38.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="3"/>
-      <c r="C57" s="116" t="s">
-        <v>94</v>
-      </c>
-      <c r="D57" s="116"/>
-      <c r="E57" s="116"/>
-      <c r="F57" s="116"/>
-      <c r="G57" s="116"/>
-      <c r="H57" s="116"/>
-      <c r="I57" s="116"/>
-      <c r="J57" s="116"/>
-      <c r="K57" s="116"/>
-      <c r="L57" s="116"/>
+      <c r="C57" s="154" t="s">
+        <v>93</v>
+      </c>
+      <c r="D57" s="154"/>
+      <c r="E57" s="154"/>
+      <c r="F57" s="154"/>
+      <c r="G57" s="154"/>
+      <c r="H57" s="154"/>
+      <c r="I57" s="154"/>
+      <c r="J57" s="154"/>
+      <c r="K57" s="154"/>
+      <c r="L57" s="154"/>
       <c r="M57" s="3"/>
     </row>
     <row r="58" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B58" s="3"/>
       <c r="C58" s="65" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
@@ -14239,7 +14333,7 @@
     <row r="59" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B59" s="3"/>
       <c r="C59" s="67" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
@@ -14255,7 +14349,7 @@
     <row r="60" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B60" s="3"/>
       <c r="C60" s="67" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
@@ -14271,7 +14365,7 @@
     <row r="61" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B61" s="3"/>
       <c r="C61" s="67" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
@@ -14287,7 +14381,7 @@
     <row r="62" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B62" s="3"/>
       <c r="C62" s="67" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
@@ -14303,7 +14397,7 @@
     <row r="63" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B63" s="3"/>
       <c r="C63" s="67" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
@@ -14383,18 +14477,18 @@
     </row>
     <row r="5" spans="2:13" ht="19" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
-      <c r="C5" s="115" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="115"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
-      <c r="H5" s="115"/>
-      <c r="I5" s="115"/>
-      <c r="J5" s="115"/>
-      <c r="K5" s="115"/>
-      <c r="L5" s="115"/>
+      <c r="C5" s="153" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="153"/>
+      <c r="E5" s="153"/>
+      <c r="F5" s="153"/>
+      <c r="G5" s="153"/>
+      <c r="H5" s="153"/>
+      <c r="I5" s="153"/>
+      <c r="J5" s="153"/>
+      <c r="K5" s="153"/>
+      <c r="L5" s="153"/>
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.2">
@@ -14414,7 +14508,7 @@
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -14430,17 +14524,17 @@
     <row r="8" spans="2:13" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="117" t="s">
-        <v>140</v>
-      </c>
-      <c r="E8" s="117"/>
-      <c r="F8" s="117"/>
-      <c r="G8" s="117"/>
-      <c r="H8" s="117"/>
-      <c r="I8" s="117"/>
-      <c r="J8" s="117"/>
-      <c r="K8" s="117"/>
-      <c r="L8" s="117"/>
+      <c r="D8" s="155" t="s">
+        <v>137</v>
+      </c>
+      <c r="E8" s="155"/>
+      <c r="F8" s="155"/>
+      <c r="G8" s="155"/>
+      <c r="H8" s="155"/>
+      <c r="I8" s="155"/>
+      <c r="J8" s="155"/>
+      <c r="K8" s="155"/>
+      <c r="L8" s="155"/>
       <c r="M8" s="3"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
@@ -14460,17 +14554,17 @@
     <row r="10" spans="2:13" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="94" t="s">
-        <v>141</v>
-      </c>
-      <c r="E10" s="94"/>
-      <c r="F10" s="94"/>
-      <c r="G10" s="94"/>
-      <c r="H10" s="94"/>
-      <c r="I10" s="94"/>
-      <c r="J10" s="94"/>
-      <c r="K10" s="94"/>
-      <c r="L10" s="94"/>
+      <c r="D10" s="128" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10" s="128"/>
+      <c r="F10" s="128"/>
+      <c r="G10" s="128"/>
+      <c r="H10" s="128"/>
+      <c r="I10" s="128"/>
+      <c r="J10" s="128"/>
+      <c r="K10" s="128"/>
+      <c r="L10" s="128"/>
       <c r="M10" s="3"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
@@ -14490,17 +14584,17 @@
     <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="94" t="s">
-        <v>104</v>
-      </c>
-      <c r="E12" s="94"/>
-      <c r="F12" s="94"/>
-      <c r="G12" s="94"/>
-      <c r="H12" s="94"/>
-      <c r="I12" s="94"/>
-      <c r="J12" s="94"/>
-      <c r="K12" s="94"/>
-      <c r="L12" s="94"/>
+      <c r="D12" s="128" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" s="128"/>
+      <c r="F12" s="128"/>
+      <c r="G12" s="128"/>
+      <c r="H12" s="128"/>
+      <c r="I12" s="128"/>
+      <c r="J12" s="128"/>
+      <c r="K12" s="128"/>
+      <c r="L12" s="128"/>
       <c r="M12" s="3"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.2">
@@ -14520,17 +14614,17 @@
     <row r="14" spans="2:13" ht="45.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="94" t="s">
-        <v>142</v>
-      </c>
-      <c r="E14" s="94"/>
-      <c r="F14" s="94"/>
-      <c r="G14" s="94"/>
-      <c r="H14" s="94"/>
-      <c r="I14" s="94"/>
-      <c r="J14" s="94"/>
-      <c r="K14" s="94"/>
-      <c r="L14" s="94"/>
+      <c r="D14" s="128" t="s">
+        <v>139</v>
+      </c>
+      <c r="E14" s="128"/>
+      <c r="F14" s="128"/>
+      <c r="G14" s="128"/>
+      <c r="H14" s="128"/>
+      <c r="I14" s="128"/>
+      <c r="J14" s="128"/>
+      <c r="K14" s="128"/>
+      <c r="L14" s="128"/>
       <c r="M14" s="3"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.2">
@@ -14550,17 +14644,17 @@
     <row r="16" spans="2:13" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="94" t="s">
-        <v>143</v>
-      </c>
-      <c r="E16" s="94"/>
-      <c r="F16" s="94"/>
-      <c r="G16" s="94"/>
-      <c r="H16" s="94"/>
-      <c r="I16" s="94"/>
-      <c r="J16" s="94"/>
-      <c r="K16" s="94"/>
-      <c r="L16" s="94"/>
+      <c r="D16" s="128" t="s">
+        <v>140</v>
+      </c>
+      <c r="E16" s="128"/>
+      <c r="F16" s="128"/>
+      <c r="G16" s="128"/>
+      <c r="H16" s="128"/>
+      <c r="I16" s="128"/>
+      <c r="J16" s="128"/>
+      <c r="K16" s="128"/>
+      <c r="L16" s="128"/>
       <c r="M16" s="3"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.2">
@@ -14580,17 +14674,17 @@
     <row r="18" spans="2:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="94" t="s">
-        <v>100</v>
-      </c>
-      <c r="E18" s="94"/>
-      <c r="F18" s="94"/>
-      <c r="G18" s="94"/>
-      <c r="H18" s="94"/>
-      <c r="I18" s="94"/>
-      <c r="J18" s="94"/>
-      <c r="K18" s="94"/>
-      <c r="L18" s="94"/>
+      <c r="D18" s="128" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="128"/>
+      <c r="F18" s="128"/>
+      <c r="G18" s="128"/>
+      <c r="H18" s="128"/>
+      <c r="I18" s="128"/>
+      <c r="J18" s="128"/>
+      <c r="K18" s="128"/>
+      <c r="L18" s="128"/>
       <c r="M18" s="3"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.2">
@@ -14610,17 +14704,17 @@
     <row r="20" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="94" t="s">
-        <v>144</v>
-      </c>
-      <c r="E20" s="94"/>
-      <c r="F20" s="94"/>
-      <c r="G20" s="94"/>
-      <c r="H20" s="94"/>
-      <c r="I20" s="94"/>
-      <c r="J20" s="94"/>
-      <c r="K20" s="94"/>
-      <c r="L20" s="94"/>
+      <c r="D20" s="128" t="s">
+        <v>141</v>
+      </c>
+      <c r="E20" s="128"/>
+      <c r="F20" s="128"/>
+      <c r="G20" s="128"/>
+      <c r="H20" s="128"/>
+      <c r="I20" s="128"/>
+      <c r="J20" s="128"/>
+      <c r="K20" s="128"/>
+      <c r="L20" s="128"/>
       <c r="M20" s="3"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.2">
@@ -14654,7 +14748,7 @@
     <row r="23" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B23" s="3"/>
       <c r="C23" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -14670,17 +14764,17 @@
     <row r="24" spans="2:13" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
-      <c r="D24" s="94" t="s">
-        <v>145</v>
-      </c>
-      <c r="E24" s="94"/>
-      <c r="F24" s="94"/>
-      <c r="G24" s="94"/>
-      <c r="H24" s="94"/>
-      <c r="I24" s="94"/>
-      <c r="J24" s="94"/>
-      <c r="K24" s="94"/>
-      <c r="L24" s="94"/>
+      <c r="D24" s="128" t="s">
+        <v>142</v>
+      </c>
+      <c r="E24" s="128"/>
+      <c r="F24" s="128"/>
+      <c r="G24" s="128"/>
+      <c r="H24" s="128"/>
+      <c r="I24" s="128"/>
+      <c r="J24" s="128"/>
+      <c r="K24" s="128"/>
+      <c r="L24" s="128"/>
       <c r="M24" s="3"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.2">
@@ -14700,17 +14794,17 @@
     <row r="26" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="94" t="s">
-        <v>146</v>
-      </c>
-      <c r="E26" s="94"/>
-      <c r="F26" s="94"/>
-      <c r="G26" s="94"/>
-      <c r="H26" s="94"/>
-      <c r="I26" s="94"/>
-      <c r="J26" s="94"/>
-      <c r="K26" s="94"/>
-      <c r="L26" s="94"/>
+      <c r="D26" s="128" t="s">
+        <v>143</v>
+      </c>
+      <c r="E26" s="128"/>
+      <c r="F26" s="128"/>
+      <c r="G26" s="128"/>
+      <c r="H26" s="128"/>
+      <c r="I26" s="128"/>
+      <c r="J26" s="128"/>
+      <c r="K26" s="128"/>
+      <c r="L26" s="128"/>
       <c r="M26" s="3"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.2">
@@ -14730,17 +14824,17 @@
     <row r="28" spans="2:13" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="94" t="s">
-        <v>101</v>
-      </c>
-      <c r="E28" s="94"/>
-      <c r="F28" s="94"/>
-      <c r="G28" s="94"/>
-      <c r="H28" s="94"/>
-      <c r="I28" s="94"/>
-      <c r="J28" s="94"/>
-      <c r="K28" s="94"/>
-      <c r="L28" s="94"/>
+      <c r="D28" s="128" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" s="128"/>
+      <c r="F28" s="128"/>
+      <c r="G28" s="128"/>
+      <c r="H28" s="128"/>
+      <c r="I28" s="128"/>
+      <c r="J28" s="128"/>
+      <c r="K28" s="128"/>
+      <c r="L28" s="128"/>
       <c r="M28" s="3"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.2">
@@ -14760,17 +14854,17 @@
     <row r="30" spans="2:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="94" t="s">
-        <v>51</v>
-      </c>
-      <c r="E30" s="94"/>
-      <c r="F30" s="94"/>
-      <c r="G30" s="94"/>
-      <c r="H30" s="94"/>
-      <c r="I30" s="94"/>
-      <c r="J30" s="94"/>
-      <c r="K30" s="94"/>
-      <c r="L30" s="94"/>
+      <c r="D30" s="128" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="128"/>
+      <c r="F30" s="128"/>
+      <c r="G30" s="128"/>
+      <c r="H30" s="128"/>
+      <c r="I30" s="128"/>
+      <c r="J30" s="128"/>
+      <c r="K30" s="128"/>
+      <c r="L30" s="128"/>
       <c r="M30" s="3"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.2">
@@ -14845,11 +14939,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C5:L5"/>
-    <mergeCell ref="D20:L20"/>
-    <mergeCell ref="D8:L8"/>
-    <mergeCell ref="D10:L10"/>
-    <mergeCell ref="D26:L26"/>
     <mergeCell ref="D30:L30"/>
     <mergeCell ref="D14:L14"/>
     <mergeCell ref="D12:L12"/>
@@ -14857,6 +14946,11 @@
     <mergeCell ref="D16:L16"/>
     <mergeCell ref="D24:L24"/>
     <mergeCell ref="D28:L28"/>
+    <mergeCell ref="C5:L5"/>
+    <mergeCell ref="D20:L20"/>
+    <mergeCell ref="D8:L8"/>
+    <mergeCell ref="D10:L10"/>
+    <mergeCell ref="D26:L26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
phase 1 tool updates
</commit_message>
<xml_diff>
--- a/Phase 1/MADMC B19 Pregancy Outcome Estimate Tool.xlsx
+++ b/Phase 1/MADMC B19 Pregancy Outcome Estimate Tool.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ritesh/Desktop/parvo-b19-modeling/Phase 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3CFB3DE-DF7C-0546-9A4D-29BB4506659A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F712ED7-8900-5746-9651-FC48907531DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="2" r:id="rId1"/>
@@ -348,9 +348,6 @@
     </r>
   </si>
   <si>
-    <t>*One-way sensitivity analyses vary just one parameter value and keeps all other parameters at base case values.</t>
-  </si>
-  <si>
     <t>Parameter</t>
   </si>
   <si>
@@ -1875,6 +1872,9 @@
   </si>
   <si>
     <t>Estimated Number of Severe Outcomes due to Parvovirus B19</t>
+  </si>
+  <si>
+    <t>*One-way sensitivity analyses vary just one parameter value and keeps all other parameters at base case values. Varied Immunity in Table 2.</t>
   </si>
 </sst>
 </file>
@@ -3923,7 +3923,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -5336,15 +5336,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>611012</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>5643</xdr:rowOff>
+      <xdr:colOff>611011</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>174976</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>502356</xdr:colOff>
+      <xdr:colOff>502355</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>52916</xdr:rowOff>
+      <xdr:rowOff>24693</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5663,7 +5663,7 @@
     <row r="6" spans="2:12" ht="32" x14ac:dyDescent="0.2">
       <c r="B6" s="18"/>
       <c r="C6" s="79" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="90"/>
@@ -5714,7 +5714,7 @@
     <row r="11" spans="2:12" ht="66" x14ac:dyDescent="0.2">
       <c r="B11" s="18"/>
       <c r="C11" s="81" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D11" s="76"/>
       <c r="E11" s="92"/>
@@ -5742,7 +5742,7 @@
     <row r="13" spans="2:12" ht="44" x14ac:dyDescent="0.2">
       <c r="B13" s="18"/>
       <c r="C13" s="81" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D13" s="76"/>
       <c r="E13" s="92"/>
@@ -5783,7 +5783,7 @@
     <row r="16" spans="2:12" ht="21" x14ac:dyDescent="0.2">
       <c r="B16" s="18"/>
       <c r="C16" s="82" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D16" s="76"/>
       <c r="E16" s="92"/>
@@ -5798,7 +5798,7 @@
     <row r="17" spans="2:12" ht="23" x14ac:dyDescent="0.2">
       <c r="B17" s="18"/>
       <c r="C17" s="81" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D17" s="76"/>
       <c r="E17" s="92"/>
@@ -5812,7 +5812,7 @@
     <row r="18" spans="2:12" ht="23" x14ac:dyDescent="0.2">
       <c r="B18" s="18"/>
       <c r="C18" s="81" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D18" s="76"/>
       <c r="E18" s="92"/>
@@ -5826,7 +5826,7 @@
     <row r="19" spans="2:12" ht="23" x14ac:dyDescent="0.2">
       <c r="B19" s="18"/>
       <c r="C19" s="81" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D19" s="76"/>
       <c r="E19" s="92"/>
@@ -5845,7 +5845,7 @@
     <row r="21" spans="2:12" ht="110" x14ac:dyDescent="0.2">
       <c r="B21" s="18"/>
       <c r="C21" s="81" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D21" s="76"/>
       <c r="E21" s="92"/>
@@ -5929,7 +5929,7 @@
     <row r="31" spans="2:12" ht="220" x14ac:dyDescent="0.2">
       <c r="B31" s="18"/>
       <c r="C31" s="81" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D31" s="76"/>
       <c r="E31" s="92"/>
@@ -5949,7 +5949,7 @@
     <row r="33" spans="2:12" ht="154" x14ac:dyDescent="0.2">
       <c r="B33" s="18"/>
       <c r="C33" s="81" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D33" s="76"/>
       <c r="E33" s="92"/>
@@ -5977,7 +5977,7 @@
     <row r="35" spans="2:12" ht="21" x14ac:dyDescent="0.2">
       <c r="B35" s="18"/>
       <c r="C35" s="82" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D35" s="76"/>
       <c r="E35" s="92"/>
@@ -6002,7 +6002,7 @@
     <row r="38" spans="2:12" ht="44" x14ac:dyDescent="0.2">
       <c r="B38" s="11"/>
       <c r="C38" s="86" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D38" s="77"/>
       <c r="E38" s="92"/>
@@ -6022,7 +6022,7 @@
     <row r="40" spans="2:12" ht="88" x14ac:dyDescent="0.2">
       <c r="B40" s="11"/>
       <c r="C40" s="86" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D40" s="78"/>
     </row>
@@ -6034,14 +6034,14 @@
     <row r="42" spans="2:12" ht="21" x14ac:dyDescent="0.2">
       <c r="B42" s="11"/>
       <c r="C42" s="87" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D42" s="11"/>
     </row>
     <row r="43" spans="2:12" ht="21" x14ac:dyDescent="0.2">
       <c r="B43" s="11"/>
       <c r="C43" s="88" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D43" s="11"/>
     </row>
@@ -6053,14 +6053,14 @@
     <row r="45" spans="2:12" ht="21" x14ac:dyDescent="0.2">
       <c r="B45" s="11"/>
       <c r="C45" s="85" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D45" s="11"/>
     </row>
     <row r="46" spans="2:12" ht="21" x14ac:dyDescent="0.2">
       <c r="B46" s="11"/>
       <c r="C46" s="85" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D46" s="11"/>
     </row>
@@ -6079,8 +6079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4E0B51A-7E99-B445-9709-9B3BD93CABEF}">
   <dimension ref="A1:AC49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AB25" sqref="AB25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6096,7 +6096,7 @@
   <sheetData>
     <row r="1" spans="1:29" s="26" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="B1" s="158" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C1" s="25"/>
       <c r="E1" s="27"/>
@@ -6113,7 +6113,7 @@
     </row>
     <row r="4" spans="1:29" ht="21" x14ac:dyDescent="0.25">
       <c r="B4" s="130" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C4" s="130"/>
       <c r="D4" s="130"/>
@@ -6156,7 +6156,7 @@
     <row r="7" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="3"/>
@@ -6183,7 +6183,7 @@
         <v>21</v>
       </c>
       <c r="C8" s="108" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D8" s="104" t="s">
         <v>14</v>
@@ -6217,7 +6217,7 @@
     <row r="9" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="109" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C9" s="107">
         <v>3600000</v>
@@ -6251,7 +6251,7 @@
     <row r="10" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="57" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C10" s="72">
         <v>0.5</v>
@@ -6285,7 +6285,7 @@
     <row r="11" spans="1:29" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="57" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C11" s="72">
         <v>0.01</v>
@@ -6319,7 +6319,7 @@
     <row r="12" spans="1:29" ht="50" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="57" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C12" s="72">
         <v>7.4999999999999997E-2</v>
@@ -6353,7 +6353,7 @@
     <row r="13" spans="1:29" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="157" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C13" s="157"/>
       <c r="D13" s="157"/>
@@ -6415,7 +6415,7 @@
     <row r="16" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="3"/>
@@ -6437,7 +6437,7 @@
     <row r="17" spans="1:18" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="155" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C17" s="110" t="s">
         <v>6</v>
@@ -6466,7 +6466,7 @@
       <c r="A18" s="3"/>
       <c r="B18" s="156"/>
       <c r="C18" s="111" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" s="111" t="s">
         <v>9</v>
@@ -6495,7 +6495,7 @@
     <row r="19" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="114" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C19" s="114">
         <f>C9*C10</f>
@@ -6532,19 +6532,19 @@
     <row r="20" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="57" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C20" s="57">
         <f>C19*C11</f>
         <v>18000</v>
       </c>
       <c r="D20" s="116">
-        <f>C19*D11</f>
-        <v>9000</v>
+        <f>D19*C11</f>
+        <v>21600</v>
       </c>
       <c r="E20" s="102">
-        <f>C19*E11</f>
-        <v>36000</v>
+        <f>E19*C11</f>
+        <v>14400</v>
       </c>
       <c r="F20" s="102">
         <f>F19*D11</f>
@@ -6569,19 +6569,19 @@
     <row r="21" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="57" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C21" s="57">
         <f>C20*C12</f>
         <v>1350</v>
       </c>
       <c r="D21" s="116">
-        <f>C20*D12</f>
-        <v>900</v>
+        <f>D20*C12</f>
+        <v>1620</v>
       </c>
       <c r="E21" s="102">
-        <f>C20*E12</f>
-        <v>1800</v>
+        <f>E20*C12</f>
+        <v>1080</v>
       </c>
       <c r="F21" s="102">
         <f>F20*D12</f>
@@ -6606,7 +6606,7 @@
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="41" t="s">
-        <v>33</v>
+        <v>149</v>
       </c>
       <c r="C22" s="41"/>
       <c r="D22" s="3"/>
@@ -6628,7 +6628,7 @@
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="41"/>
       <c r="D23" s="40"/>
@@ -6650,7 +6650,7 @@
     <row r="24" spans="1:18" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="128" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="128"/>
       <c r="D24" s="128"/>
@@ -6672,7 +6672,7 @@
     <row r="25" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="128" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" s="128"/>
       <c r="D25" s="128"/>
@@ -7045,17 +7045,17 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B44" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B45" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B46" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C46" s="45" t="s">
         <v>14</v>
@@ -7075,7 +7075,7 @@
     </row>
     <row r="47" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="B47" s="42" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C47" s="43">
         <f>F47-E47</f>
@@ -7100,7 +7100,7 @@
     </row>
     <row r="48" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="B48" s="42" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C48" s="43">
         <f>F48-E48</f>
@@ -7125,7 +7125,7 @@
     </row>
     <row r="49" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B49" s="42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C49" s="43">
         <f>F49-E49</f>
@@ -7165,6 +7165,7 @@
     <mergeCell ref="F17:G17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -7174,7 +7175,7 @@
   <dimension ref="B1:AH128"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7217,7 +7218,7 @@
     </row>
     <row r="3" spans="2:34" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="133" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D3" s="133"/>
       <c r="E3" s="133"/>
@@ -7239,7 +7240,7 @@
     <row r="6" spans="2:34" ht="26.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -7326,7 +7327,7 @@
     <row r="8" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="112" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="47">
         <v>3600000</v>
@@ -7334,7 +7335,7 @@
       <c r="E8" s="49"/>
       <c r="F8" s="3"/>
       <c r="G8" s="135" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H8" s="13">
         <v>0.75</v>
@@ -7424,10 +7425,10 @@
     <row r="9" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
       <c r="C9" s="103" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D9" s="106" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" s="50"/>
       <c r="F9" s="3"/>
@@ -7520,7 +7521,7 @@
     <row r="10" spans="2:34" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="103" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D10" s="106" t="s">
         <v>13</v>
@@ -7616,7 +7617,7 @@
     <row r="11" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
       <c r="C11" s="103" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D11" s="117">
         <v>7.4999999999999997E-2</v>
@@ -7990,7 +7991,7 @@
     <row r="15" spans="2:34" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="136" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D15" s="137"/>
       <c r="E15" s="48"/>
@@ -8176,7 +8177,7 @@
     <row r="17" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="3"/>
       <c r="C17" s="139" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D17" s="140"/>
       <c r="E17" s="36"/>
@@ -8270,7 +8271,7 @@
     <row r="18" spans="2:34" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="139" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D18" s="140"/>
       <c r="E18" s="36"/>
@@ -8449,7 +8450,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="144" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J20" s="144"/>
       <c r="K20" s="144"/>
@@ -8508,7 +8509,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -8567,7 +8568,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -8859,7 +8860,7 @@
       <c r="E27" s="48"/>
       <c r="F27" s="3"/>
       <c r="G27" s="135" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H27" s="13">
         <v>1</v>
@@ -9962,7 +9963,7 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="144" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J39" s="144"/>
       <c r="K39" s="144"/>
@@ -13588,7 +13589,7 @@
   <sheetData>
     <row r="4" spans="2:13" ht="19" x14ac:dyDescent="0.25">
       <c r="B4" s="150" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" s="150"/>
       <c r="D4" s="150"/>
@@ -13619,7 +13620,7 @@
     <row r="6" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
       <c r="C6" s="65" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -13635,7 +13636,7 @@
     <row r="7" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="3"/>
       <c r="C7" s="65" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -13651,7 +13652,7 @@
     <row r="8" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="65" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -13667,7 +13668,7 @@
     <row r="9" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
       <c r="C9" s="65" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -13683,7 +13684,7 @@
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
       <c r="C10" s="66" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -13699,7 +13700,7 @@
     <row r="11" spans="2:13" ht="63.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
       <c r="C11" s="151" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" s="151"/>
       <c r="E11" s="151"/>
@@ -13715,7 +13716,7 @@
     <row r="12" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="3"/>
       <c r="C12" s="65" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -13731,7 +13732,7 @@
     <row r="13" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="3"/>
       <c r="C13" s="67" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -13747,7 +13748,7 @@
     <row r="14" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="3"/>
       <c r="C14" s="67" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -13763,7 +13764,7 @@
     <row r="15" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="3"/>
       <c r="C15" s="67" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -13779,7 +13780,7 @@
     <row r="16" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" s="3"/>
       <c r="C16" s="67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -13823,7 +13824,7 @@
     <row r="19" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
       <c r="C19" s="65" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -13839,7 +13840,7 @@
     <row r="20" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" s="3"/>
       <c r="C20" s="65" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -13855,7 +13856,7 @@
     <row r="21" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="3"/>
       <c r="C21" s="65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -13871,7 +13872,7 @@
     <row r="22" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" s="3"/>
       <c r="C22" s="65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -13887,7 +13888,7 @@
     <row r="23" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B23" s="3"/>
       <c r="C23" s="66" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -13903,7 +13904,7 @@
     <row r="24" spans="2:13" ht="60.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="3"/>
       <c r="C24" s="151" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D24" s="151"/>
       <c r="E24" s="151"/>
@@ -13919,7 +13920,7 @@
     <row r="25" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" s="3"/>
       <c r="C25" s="65" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -13935,7 +13936,7 @@
     <row r="26" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B26" s="3"/>
       <c r="C26" s="67" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -13951,7 +13952,7 @@
     <row r="27" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B27" s="3"/>
       <c r="C27" s="67" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -13995,7 +13996,7 @@
     <row r="30" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B30" s="3"/>
       <c r="C30" s="65" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -14011,7 +14012,7 @@
     <row r="31" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B31" s="3"/>
       <c r="C31" s="65" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -14027,7 +14028,7 @@
     <row r="32" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B32" s="3"/>
       <c r="C32" s="65" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -14043,7 +14044,7 @@
     <row r="33" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B33" s="3"/>
       <c r="C33" s="65" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -14059,7 +14060,7 @@
     <row r="34" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B34" s="3"/>
       <c r="C34" s="66" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
@@ -14075,7 +14076,7 @@
     <row r="35" spans="2:13" ht="51.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="3"/>
       <c r="C35" s="151" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D35" s="151"/>
       <c r="E35" s="151"/>
@@ -14091,7 +14092,7 @@
     <row r="36" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B36" s="3"/>
       <c r="C36" s="65" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
@@ -14107,7 +14108,7 @@
     <row r="37" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B37" s="3"/>
       <c r="C37" s="67" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
@@ -14123,7 +14124,7 @@
     <row r="38" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B38" s="3"/>
       <c r="C38" s="67" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
@@ -14167,7 +14168,7 @@
     <row r="41" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" s="3"/>
       <c r="C41" s="65" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
@@ -14183,7 +14184,7 @@
     <row r="42" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B42" s="3"/>
       <c r="C42" s="65" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
@@ -14199,7 +14200,7 @@
     <row r="43" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B43" s="3"/>
       <c r="C43" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
@@ -14215,7 +14216,7 @@
     <row r="44" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B44" s="3"/>
       <c r="C44" s="65" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
@@ -14231,7 +14232,7 @@
     <row r="45" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B45" s="3"/>
       <c r="C45" s="66" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
@@ -14247,7 +14248,7 @@
     <row r="46" spans="2:13" ht="54.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="3"/>
       <c r="C46" s="151" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D46" s="151"/>
       <c r="E46" s="151"/>
@@ -14263,7 +14264,7 @@
     <row r="47" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B47" s="3"/>
       <c r="C47" s="65" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
@@ -14279,7 +14280,7 @@
     <row r="48" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B48" s="3"/>
       <c r="C48" s="67" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D48" s="68"/>
       <c r="E48" s="68"/>
@@ -14295,7 +14296,7 @@
     <row r="49" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B49" s="3"/>
       <c r="C49" s="67" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
@@ -14339,7 +14340,7 @@
     <row r="52" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B52" s="3"/>
       <c r="C52" s="65" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
@@ -14355,7 +14356,7 @@
     <row r="53" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B53" s="3"/>
       <c r="C53" s="65" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
@@ -14371,7 +14372,7 @@
     <row r="54" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B54" s="3"/>
       <c r="C54" s="65" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
@@ -14387,7 +14388,7 @@
     <row r="55" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B55" s="3"/>
       <c r="C55" s="65" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
@@ -14403,7 +14404,7 @@
     <row r="56" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B56" s="3"/>
       <c r="C56" s="66" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
@@ -14419,7 +14420,7 @@
     <row r="57" spans="2:13" ht="38.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="3"/>
       <c r="C57" s="151" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D57" s="151"/>
       <c r="E57" s="151"/>
@@ -14435,7 +14436,7 @@
     <row r="58" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B58" s="3"/>
       <c r="C58" s="65" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
@@ -14451,7 +14452,7 @@
     <row r="59" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B59" s="3"/>
       <c r="C59" s="67" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
@@ -14467,7 +14468,7 @@
     <row r="60" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B60" s="3"/>
       <c r="C60" s="67" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
@@ -14483,7 +14484,7 @@
     <row r="61" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B61" s="3"/>
       <c r="C61" s="67" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
@@ -14499,7 +14500,7 @@
     <row r="62" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B62" s="3"/>
       <c r="C62" s="67" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
@@ -14515,7 +14516,7 @@
     <row r="63" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B63" s="3"/>
       <c r="C63" s="67" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
@@ -14596,7 +14597,7 @@
     <row r="5" spans="2:13" ht="19" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="150" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" s="150"/>
       <c r="E5" s="150"/>
@@ -14626,7 +14627,7 @@
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -14643,7 +14644,7 @@
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="152" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E8" s="152"/>
       <c r="F8" s="152"/>
@@ -14673,7 +14674,7 @@
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="131" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E10" s="131"/>
       <c r="F10" s="131"/>
@@ -14703,7 +14704,7 @@
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="131" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E12" s="131"/>
       <c r="F12" s="131"/>
@@ -14733,7 +14734,7 @@
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="131" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E14" s="131"/>
       <c r="F14" s="131"/>
@@ -14763,7 +14764,7 @@
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="131" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E16" s="131"/>
       <c r="F16" s="131"/>
@@ -14793,7 +14794,7 @@
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="131" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E18" s="131"/>
       <c r="F18" s="131"/>
@@ -14823,7 +14824,7 @@
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="131" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E20" s="131"/>
       <c r="F20" s="131"/>
@@ -14866,7 +14867,7 @@
     <row r="23" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B23" s="3"/>
       <c r="C23" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -14883,7 +14884,7 @@
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
       <c r="D24" s="131" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E24" s="131"/>
       <c r="F24" s="131"/>
@@ -14913,7 +14914,7 @@
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="131" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E26" s="131"/>
       <c r="F26" s="131"/>
@@ -14943,7 +14944,7 @@
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="131" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E28" s="131"/>
       <c r="F28" s="131"/>
@@ -14973,7 +14974,7 @@
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="131" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E30" s="131"/>
       <c r="F30" s="131"/>

</xml_diff>